<commit_message>
Alteração do Excel do SIGAA
</commit_message>
<xml_diff>
--- a/Arquivos/prazo.xlsx
+++ b/Arquivos/prazo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herso\OneDrive\APython\Exercícios\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{135591F0-F8C6-4AEB-8DC3-4736717A5AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BA1552-BB8B-4AD8-A694-AD912AC6627D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840"/>
+    <workbookView xWindow="17280" yWindow="0" windowWidth="21120" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="202">
   <si>
     <t>UNIVERSIDADE FEDERAL DA PARAÍBA</t>
   </si>
@@ -335,9 +335,6 @@
     <t>LEYS EDUARDO DOS SANTOS SOARES</t>
   </si>
   <si>
-    <t>Pág. 1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> de 3</t>
   </si>
   <si>
@@ -632,12 +629,15 @@
   </si>
   <si>
     <t>Pág. 3</t>
+  </si>
+  <si>
+    <t>* Uma observação, essa colunas marcadas, são número 13 e 14 respectivamente. Deve ser por conta das células minimizadas nesse arquivo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="10"/>
@@ -680,7 +680,7 @@
       <name val="sansserif"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,6 +696,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="31"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -721,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -738,15 +744,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -760,32 +785,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1227,10 +1251,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12:O12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1245,7 +1271,7 @@
     <col min="9" max="9" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" customWidth="1"/>
     <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="1.28515625" bestFit="1" customWidth="1"/>
@@ -1256,13 +1282,13 @@
     <col min="24" max="24" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="0.95" customHeight="1">
+    <row r="1" spans="1:37" ht="0.95" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1282,107 +1308,107 @@
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
     </row>
-    <row r="2" spans="1:24" ht="15" customHeight="1">
+    <row r="2" spans="1:37" ht="15" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:37" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
     </row>
-    <row r="4" spans="1:24" ht="6.95" customHeight="1">
+    <row r="4" spans="1:37" ht="6.95" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
-    <row r="5" spans="1:24" ht="8.1" customHeight="1">
+    <row r="5" spans="1:37" ht="8.1" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1392,57 +1418,57 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
     </row>
-    <row r="6" spans="1:24" ht="18.95" customHeight="1">
+    <row r="6" spans="1:37" ht="18.95" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
       <c r="X6" s="1"/>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1">
+    <row r="7" spans="1:37" ht="15" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="11" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -1450,29 +1476,29 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1">
+    <row r="8" spans="1:37" ht="15" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="11" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -1480,74 +1506,74 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
-    <row r="9" spans="1:24" ht="0.95" customHeight="1">
+    <row r="9" spans="1:37" ht="0.95" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
-    <row r="10" spans="1:24" ht="39.950000000000003" customHeight="1">
+    <row r="10" spans="1:37" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
-    <row r="11" spans="1:24" ht="18" customHeight="1">
+    <row r="11" spans="1:37" ht="18" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1563,33 +1589,33 @@
       <c r="N11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="7"/>
+      <c r="O11" s="9"/>
       <c r="P11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
-    <row r="12" spans="1:24" ht="24" customHeight="1">
+    <row r="12" spans="1:37" ht="24" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="18" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="4" t="s">
         <v>19</v>
       </c>
@@ -1599,39 +1625,54 @@
       <c r="L12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="N12" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="7"/>
-      <c r="P12" s="18" t="s">
+      <c r="O12" s="27"/>
+      <c r="P12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-    </row>
-    <row r="13" spans="1:24" ht="24" customHeight="1">
+      <c r="X12" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
+      <c r="AC12" s="29"/>
+      <c r="AD12" s="29"/>
+      <c r="AE12" s="29"/>
+      <c r="AF12" s="29"/>
+      <c r="AG12" s="29"/>
+      <c r="AH12" s="29"/>
+      <c r="AI12" s="29"/>
+      <c r="AJ12" s="29"/>
+      <c r="AK12" s="29"/>
+    </row>
+    <row r="13" spans="1:37" ht="24" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="18" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1644,36 +1685,36 @@
       <c r="M13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="19" t="s">
+      <c r="N13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O13" s="7"/>
-      <c r="P13" s="18" t="s">
+      <c r="O13" s="9"/>
+      <c r="P13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
     </row>
-    <row r="14" spans="1:24" ht="24" customHeight="1">
+    <row r="14" spans="1:37" ht="24" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="18" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1686,36 +1727,36 @@
       <c r="M14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="19" t="s">
+      <c r="N14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="7"/>
-      <c r="P14" s="18" t="s">
+      <c r="O14" s="9"/>
+      <c r="P14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
     </row>
-    <row r="15" spans="1:24" ht="24" customHeight="1">
+    <row r="15" spans="1:37" ht="24" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="18" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1728,36 +1769,36 @@
       <c r="M15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="N15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="7"/>
-      <c r="P15" s="18" t="s">
+      <c r="O15" s="9"/>
+      <c r="P15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
     </row>
-    <row r="16" spans="1:24" ht="24" customHeight="1">
+    <row r="16" spans="1:37" ht="24" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="18" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="4" t="s">
         <v>40</v>
       </c>
@@ -1770,18 +1811,18 @@
       <c r="M16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="N16" s="19" t="s">
+      <c r="N16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O16" s="7"/>
-      <c r="P16" s="18" t="s">
+      <c r="O16" s="9"/>
+      <c r="P16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -1790,16 +1831,16 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="18" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
       <c r="J17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1812,18 +1853,18 @@
       <c r="M17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N17" s="19" t="s">
+      <c r="N17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="O17" s="7"/>
-      <c r="P17" s="18" t="s">
+      <c r="O17" s="9"/>
+      <c r="P17" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -1832,16 +1873,16 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="18" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="4" t="s">
         <v>52</v>
       </c>
@@ -1854,18 +1895,18 @@
       <c r="M18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="19" t="s">
+      <c r="N18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="O18" s="7"/>
-      <c r="P18" s="18" t="s">
+      <c r="O18" s="9"/>
+      <c r="P18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
@@ -1874,16 +1915,16 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="18" t="s">
+      <c r="E19" s="9"/>
+      <c r="F19" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="4" t="s">
         <v>52</v>
       </c>
@@ -1896,18 +1937,18 @@
       <c r="M19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N19" s="19" t="s">
+      <c r="N19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="18" t="s">
+      <c r="O19" s="9"/>
+      <c r="P19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
@@ -1916,16 +1957,16 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="18" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="4" t="s">
         <v>60</v>
       </c>
@@ -1938,18 +1979,18 @@
       <c r="M20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="N20" s="19" t="s">
+      <c r="N20" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="O20" s="7"/>
-      <c r="P20" s="18" t="s">
+      <c r="O20" s="9"/>
+      <c r="P20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
@@ -1958,16 +1999,16 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="18" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="4" t="s">
         <v>32</v>
       </c>
@@ -1980,18 +2021,18 @@
       <c r="M21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N21" s="19" t="s">
+      <c r="N21" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O21" s="7"/>
-      <c r="P21" s="18" t="s">
+      <c r="O21" s="9"/>
+      <c r="P21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
@@ -2000,16 +2041,16 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="18" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
       <c r="J22" s="4" t="s">
         <v>68</v>
       </c>
@@ -2022,18 +2063,18 @@
       <c r="M22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="N22" s="19" t="s">
+      <c r="N22" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="O22" s="7"/>
-      <c r="P22" s="18" t="s">
+      <c r="O22" s="9"/>
+      <c r="P22" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
@@ -2042,16 +2083,16 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="18" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="4" t="s">
         <v>26</v>
       </c>
@@ -2064,18 +2105,18 @@
       <c r="M23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N23" s="19" t="s">
+      <c r="N23" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O23" s="7"/>
-      <c r="P23" s="18" t="s">
+      <c r="O23" s="9"/>
+      <c r="P23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
@@ -2084,16 +2125,16 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="18" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="4" t="s">
         <v>76</v>
       </c>
@@ -2106,18 +2147,18 @@
       <c r="M24" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N24" s="19" t="s">
+      <c r="N24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="O24" s="7"/>
-      <c r="P24" s="18" t="s">
+      <c r="O24" s="9"/>
+      <c r="P24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
@@ -2126,16 +2167,16 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="18" t="s">
+      <c r="E25" s="9"/>
+      <c r="F25" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="4" t="s">
         <v>19</v>
       </c>
@@ -2148,18 +2189,18 @@
       <c r="M25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N25" s="19" t="s">
+      <c r="N25" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="7"/>
-      <c r="P25" s="18" t="s">
+      <c r="O25" s="9"/>
+      <c r="P25" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -2168,16 +2209,16 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="18" t="s">
+      <c r="E26" s="9"/>
+      <c r="F26" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="4" t="s">
         <v>40</v>
       </c>
@@ -2190,18 +2231,18 @@
       <c r="M26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="N26" s="19" t="s">
+      <c r="N26" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O26" s="7"/>
-      <c r="P26" s="18" t="s">
+      <c r="O26" s="9"/>
+      <c r="P26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-      <c r="U26" s="7"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
@@ -2210,16 +2251,16 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="18" t="s">
+      <c r="E27" s="9"/>
+      <c r="F27" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="4" t="s">
         <v>86</v>
       </c>
@@ -2232,18 +2273,18 @@
       <c r="M27" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="N27" s="19" t="s">
+      <c r="N27" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="O27" s="7"/>
-      <c r="P27" s="18" t="s">
+      <c r="O27" s="9"/>
+      <c r="P27" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
@@ -2252,16 +2293,16 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="18" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="4" t="s">
         <v>32</v>
       </c>
@@ -2274,18 +2315,18 @@
       <c r="M28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N28" s="19" t="s">
+      <c r="N28" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O28" s="7"/>
-      <c r="P28" s="18" t="s">
+      <c r="O28" s="9"/>
+      <c r="P28" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
@@ -2294,16 +2335,16 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="18" t="s">
+      <c r="E29" s="9"/>
+      <c r="F29" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
       <c r="J29" s="4" t="s">
         <v>76</v>
       </c>
@@ -2316,18 +2357,18 @@
       <c r="M29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N29" s="19" t="s">
+      <c r="N29" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="O29" s="7"/>
-      <c r="P29" s="18" t="s">
+      <c r="O29" s="9"/>
+      <c r="P29" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
@@ -2336,16 +2377,16 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="18" t="s">
+      <c r="E30" s="9"/>
+      <c r="F30" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="4" t="s">
         <v>32</v>
       </c>
@@ -2358,18 +2399,18 @@
       <c r="M30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N30" s="19" t="s">
+      <c r="N30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O30" s="7"/>
-      <c r="P30" s="18" t="s">
+      <c r="O30" s="9"/>
+      <c r="P30" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
@@ -2378,16 +2419,16 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="18" t="s">
+      <c r="E31" s="9"/>
+      <c r="F31" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
       <c r="J31" s="4" t="s">
         <v>19</v>
       </c>
@@ -2400,18 +2441,18 @@
       <c r="M31" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N31" s="19" t="s">
+      <c r="N31" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O31" s="7"/>
-      <c r="P31" s="18" t="s">
+      <c r="O31" s="9"/>
+      <c r="P31" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
@@ -2420,16 +2461,16 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="18" t="s">
+      <c r="E32" s="9"/>
+      <c r="F32" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
       <c r="J32" s="4" t="s">
         <v>40</v>
       </c>
@@ -2442,18 +2483,18 @@
       <c r="M32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="N32" s="19" t="s">
+      <c r="N32" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O32" s="7"/>
-      <c r="P32" s="18" t="s">
+      <c r="O32" s="9"/>
+      <c r="P32" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
@@ -2462,16 +2503,16 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="18" t="s">
+      <c r="E33" s="9"/>
+      <c r="F33" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
       <c r="J33" s="4" t="s">
         <v>52</v>
       </c>
@@ -2484,68 +2525,140 @@
       <c r="M33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N33" s="19" t="s">
+      <c r="N33" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="O33" s="7"/>
-      <c r="P33" s="18" t="s">
+      <c r="O33" s="9"/>
+      <c r="P33" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
     </row>
-    <row r="34" spans="1:24" ht="15.95" customHeight="1">
+    <row r="34" spans="1:24" s="6" customFormat="1" ht="24" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="6" t="s">
+      <c r="C34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="U34" s="7"/>
-      <c r="V34" s="7"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
+      <c r="D34" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="106">
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="P33:U33"/>
-    <mergeCell ref="O34:S34"/>
-    <mergeCell ref="T34:V34"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:U31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="P32:U32"/>
+  <mergeCells count="108">
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="I8:R8"/>
+    <mergeCell ref="C9:V9"/>
+    <mergeCell ref="C10:V10"/>
+    <mergeCell ref="E1:F5"/>
+    <mergeCell ref="H2:P2"/>
+    <mergeCell ref="R2:T4"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="H4:P5"/>
+    <mergeCell ref="D6:W6"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:U13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:U14"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:U11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:U12"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P17:U17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:U18"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P15:U15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:U16"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:U21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:U22"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:U19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:U20"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:U25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:U26"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:U23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:U24"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:I29"/>
     <mergeCell ref="N29:O29"/>
@@ -2562,82 +2675,20 @@
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="P28:U28"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:U25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:U26"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:U23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:U24"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:U21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:U22"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:U19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:U20"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P17:U17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:U18"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:U15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:U16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:U13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:U14"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:U11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:U12"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="I8:R8"/>
-    <mergeCell ref="C9:V9"/>
-    <mergeCell ref="C10:V10"/>
-    <mergeCell ref="E1:F5"/>
-    <mergeCell ref="H2:P2"/>
-    <mergeCell ref="R2:T4"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="H4:P5"/>
-    <mergeCell ref="D6:W6"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="P33:U33"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:U31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="P32:U32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="P34:T34"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2647,10 +2698,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2671,21 +2724,21 @@
   <sheetData>
     <row r="1" spans="1:15" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1">
@@ -2712,12 +2765,12 @@
       <c r="I2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
@@ -2725,10 +2778,10 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>32</v>
@@ -2742,15 +2795,15 @@
       <c r="H3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="18" t="s">
+      <c r="I3" s="30">
+        <v>44958</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
@@ -2758,10 +2811,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>60</v>
@@ -2775,15 +2828,15 @@
       <c r="H4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="18" t="s">
+      <c r="J4" s="9"/>
+      <c r="K4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
@@ -2791,10 +2844,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>60</v>
@@ -2808,15 +2861,15 @@
       <c r="H5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
@@ -2824,10 +2877,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>32</v>
@@ -2841,15 +2894,15 @@
       <c r="H6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="18" t="s">
+      <c r="J6" s="9"/>
+      <c r="K6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
@@ -2857,10 +2910,10 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>76</v>
@@ -2874,15 +2927,15 @@
       <c r="H7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="18" t="s">
+      <c r="J7" s="9"/>
+      <c r="K7" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
@@ -2890,10 +2943,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>40</v>
@@ -2907,15 +2960,15 @@
       <c r="H8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="18" t="s">
+      <c r="J8" s="9"/>
+      <c r="K8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
@@ -2923,10 +2976,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>19</v>
@@ -2940,15 +2993,15 @@
       <c r="H9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="18" t="s">
+      <c r="J9" s="9"/>
+      <c r="K9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
@@ -2956,10 +3009,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>32</v>
@@ -2973,15 +3026,15 @@
       <c r="H10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="18" t="s">
+      <c r="J10" s="9"/>
+      <c r="K10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
@@ -2989,10 +3042,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>40</v>
@@ -3006,15 +3059,15 @@
       <c r="H11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="18" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
@@ -3022,10 +3075,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>76</v>
@@ -3039,15 +3092,15 @@
       <c r="H12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="18" t="s">
+      <c r="J12" s="9"/>
+      <c r="K12" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
@@ -3055,10 +3108,10 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>26</v>
@@ -3072,15 +3125,15 @@
       <c r="H13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="18" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
@@ -3088,10 +3141,10 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>40</v>
@@ -3105,15 +3158,15 @@
       <c r="H14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="18" t="s">
+      <c r="J14" s="9"/>
+      <c r="K14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
@@ -3121,10 +3174,10 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>32</v>
@@ -3138,15 +3191,15 @@
       <c r="H15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="18" t="s">
+      <c r="J15" s="9"/>
+      <c r="K15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
@@ -3154,10 +3207,10 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>60</v>
@@ -3171,73 +3224,73 @@
       <c r="H16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="18" t="s">
+      <c r="J16" s="9"/>
+      <c r="K16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" ht="15.95" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="C17" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" ht="12" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="C18" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" ht="39.950000000000003" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
+      <c r="B19" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" ht="18" customHeight="1">
@@ -3264,12 +3317,12 @@
       <c r="I20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="7"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
@@ -3277,10 +3330,10 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>68</v>
@@ -3294,15 +3347,15 @@
       <c r="H21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="18" t="s">
+      <c r="J21" s="9"/>
+      <c r="K21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
@@ -3310,10 +3363,10 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>68</v>
@@ -3327,15 +3380,15 @@
       <c r="H22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="18" t="s">
+      <c r="J22" s="9"/>
+      <c r="K22" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
@@ -3343,10 +3396,10 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>32</v>
@@ -3355,20 +3408,20 @@
         <v>20</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
@@ -3376,32 +3429,32 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="4" t="s">
+      <c r="I24" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="J24" s="9"/>
+      <c r="K24" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
@@ -3409,10 +3462,10 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>68</v>
@@ -3426,15 +3479,15 @@
       <c r="H25" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I25" s="19" t="s">
+      <c r="I25" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J25" s="7"/>
-      <c r="K25" s="18" t="s">
+      <c r="J25" s="9"/>
+      <c r="K25" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
@@ -3442,32 +3495,32 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>156</v>
-      </c>
       <c r="E26" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="4" t="s">
+      <c r="I26" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I26" s="19" t="s">
+      <c r="J26" s="9"/>
+      <c r="K26" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
@@ -3475,10 +3528,10 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>68</v>
@@ -3492,15 +3545,15 @@
       <c r="H27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I27" s="19" t="s">
+      <c r="I27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J27" s="7"/>
-      <c r="K27" s="18" t="s">
+      <c r="J27" s="9"/>
+      <c r="K27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
@@ -3508,10 +3561,10 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>68</v>
@@ -3525,15 +3578,15 @@
       <c r="H28" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I28" s="19" t="s">
+      <c r="I28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="7"/>
-      <c r="K28" s="18" t="s">
+      <c r="J28" s="9"/>
+      <c r="K28" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
@@ -3541,10 +3594,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>68</v>
@@ -3558,15 +3611,15 @@
       <c r="H29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="19" t="s">
+      <c r="I29" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="J29" s="7"/>
-      <c r="K29" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
@@ -3574,32 +3627,32 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>166</v>
-      </c>
       <c r="E30" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I30" s="19" t="s">
+      <c r="J30" s="9"/>
+      <c r="K30" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J30" s="7"/>
-      <c r="K30" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
@@ -3607,10 +3660,10 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>32</v>
@@ -3624,15 +3677,15 @@
       <c r="H31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I31" s="19" t="s">
+      <c r="I31" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="18" t="s">
+      <c r="J31" s="9"/>
+      <c r="K31" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
@@ -3646,19 +3699,69 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="K32" s="7"/>
-      <c r="L32" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
+      <c r="J32" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="K32" s="9"/>
+      <c r="L32" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
       <c r="O32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="C17:M17"/>
+    <mergeCell ref="C18:L18"/>
+    <mergeCell ref="B19:N19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:M27"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="K31:M31"/>
     <mergeCell ref="J32:K32"/>
@@ -3669,56 +3772,6 @@
     <mergeCell ref="K29:M29"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="K30:M30"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="C17:M17"/>
-    <mergeCell ref="C18:L18"/>
-    <mergeCell ref="B19:N19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3727,7 +3780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -3751,21 +3804,21 @@
   <sheetData>
     <row r="1" spans="1:15" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="B1" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1">
@@ -3792,12 +3845,12 @@
       <c r="I2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
@@ -3805,32 +3858,32 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>171</v>
-      </c>
       <c r="E3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="J3" s="9"/>
+      <c r="K3" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
@@ -3838,10 +3891,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>68</v>
@@ -3855,15 +3908,15 @@
       <c r="H4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="18" t="s">
+      <c r="J4" s="9"/>
+      <c r="K4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
@@ -3871,32 +3924,32 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>175</v>
-      </c>
       <c r="E5" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="9"/>
+      <c r="K5" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
@@ -3904,32 +3957,32 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>177</v>
-      </c>
       <c r="E6" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="J6" s="9"/>
+      <c r="K6" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
@@ -3937,10 +3990,10 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>32</v>
@@ -3954,15 +4007,15 @@
       <c r="H7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="18" t="s">
+      <c r="J7" s="9"/>
+      <c r="K7" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
@@ -3970,32 +4023,32 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>181</v>
-      </c>
       <c r="E8" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="J8" s="9"/>
+      <c r="K8" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
@@ -4003,32 +4056,32 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>183</v>
-      </c>
       <c r="E9" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="J9" s="9"/>
+      <c r="K9" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
@@ -4036,32 +4089,32 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>185</v>
-      </c>
       <c r="E10" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="J10" s="9"/>
+      <c r="K10" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
@@ -4069,32 +4122,32 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>187</v>
-      </c>
       <c r="E11" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
@@ -4102,10 +4155,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>68</v>
@@ -4119,15 +4172,15 @@
       <c r="H12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
@@ -4135,32 +4188,32 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>191</v>
-      </c>
       <c r="E13" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
@@ -4168,32 +4221,32 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>193</v>
-      </c>
       <c r="E14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="J14" s="9"/>
+      <c r="K14" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
@@ -4201,10 +4254,10 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>40</v>
@@ -4218,15 +4271,15 @@
       <c r="H15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="18" t="s">
+      <c r="J15" s="9"/>
+      <c r="K15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
@@ -4234,32 +4287,32 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="E16" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="I16" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="J16" s="9"/>
+      <c r="K16" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
@@ -4267,10 +4320,10 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>32</v>
@@ -4284,52 +4337,52 @@
       <c r="H17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="18" t="s">
+      <c r="J17" s="9"/>
+      <c r="K17" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" ht="15.95" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" ht="12" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="C19" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -4344,56 +4397,56 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
+      <c r="J20" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="K20" s="9"/>
+      <c r="L20" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
       <c r="O20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:M16"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="K17:M17"/>
     <mergeCell ref="C18:M18"/>
     <mergeCell ref="C19:L19"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="L20:N20"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>